<commit_message>
Correções Junto Com o professor
</commit_message>
<xml_diff>
--- a/resources/ACE.xlsx
+++ b/resources/ACE.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gilson\Documents\Projeto_SysInventFlor\SysInventFlor\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="10545"/>
   </bookViews>
@@ -11,25 +16,36 @@
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Estratos</t>
   </si>
   <si>
     <t>Variavel</t>
   </si>
+  <si>
+    <t>Area</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -57,9 +73,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -72,6 +91,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -79,7 +101,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -117,9 +139,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -154,7 +176,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -189,7 +211,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -363,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -375,192 +397,262 @@
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>15.8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="1">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>7.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="2">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="2">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" s="1">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="2">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
       <c r="B6" s="1">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1</v>
       </c>
       <c r="B7" s="1">
         <v>16.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
       <c r="B8" s="1">
         <v>12.2</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2</v>
       </c>
       <c r="B9" s="1">
         <v>20.399999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2</v>
       </c>
       <c r="B10" s="1">
         <v>30.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2</v>
       </c>
       <c r="B11" s="1">
         <v>30.7</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2</v>
       </c>
       <c r="B12" s="1">
         <v>27.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2</v>
       </c>
       <c r="B13" s="1">
         <v>28.4</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2</v>
       </c>
       <c r="B14" s="1">
         <v>19.7</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2</v>
       </c>
       <c r="B15" s="1">
         <v>20.399999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2</v>
       </c>
       <c r="B16" s="1">
         <v>23.1</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>3</v>
       </c>
       <c r="B17" s="1">
         <v>21.3</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>3</v>
       </c>
       <c r="B18" s="1">
         <v>24.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>3</v>
       </c>
       <c r="B19" s="1">
         <v>29.2</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>3</v>
       </c>
       <c r="B20" s="1">
         <v>21.8</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>3</v>
       </c>
       <c r="B21" s="1">
         <v>33.1</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>3</v>
       </c>
       <c r="B22" s="1">
         <v>35.799999999999997</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>3</v>
       </c>
       <c r="B23" s="1">
         <v>26.7</v>
       </c>
+      <c r="C23" s="2">
+        <v>14.2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>